<commit_message>
Renaming of multiple / update forms
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-3AA.xlsx
+++ b/form_reporting_templates/Form-3AA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-reference-forms\form_reporting_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\Data dissemination\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FD234A-7FC0-4705-8A4C-1CFD3AD1BBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90D57A8-22E1-4003-97AC-E3A948942B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="dV4x4UN/0VvyFBtyDoIunEcfcYZ4v5uYvk1jvD8vzzLvThv6/Y3drfR5cofF0NFHWy380GJVRhDwCQZMDGpoHQ==" workbookSaltValue="zVm6vMVUmkQ3Bwhy95qLKQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
@@ -48,6 +48,9 @@
     <t>Full name</t>
   </si>
   <si>
+    <t>Organization</t>
+  </si>
+  <si>
     <t>General information</t>
   </si>
   <si>
@@ -84,9 +87,6 @@
     <t>Reporting entity</t>
   </si>
   <si>
-    <t>Reporting month</t>
-  </si>
-  <si>
     <t>Day of month</t>
   </si>
   <si>
@@ -126,7 +126,7 @@
     <t>Type of fate</t>
   </si>
   <si>
-    <t>Organisation</t>
+    <t>Month</t>
   </si>
   <si>
     <t>email</t>
@@ -141,10 +141,10 @@
     <t>IOTC Form 3AA | metadata</t>
   </si>
   <si>
+    <t>Flag state</t>
+  </si>
+  <si>
     <t>3AA</t>
-  </si>
-  <si>
-    <t>Flag state</t>
   </si>
 </sst>
 </file>
@@ -275,7 +275,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -727,6 +727,30 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -736,7 +760,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -940,9 +964,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -960,6 +981,24 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1380,39 +1419,39 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="87"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="91"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="88"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="90"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="94"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="32"/>
       <c r="C4" s="33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E4" s="35"/>
       <c r="F4" s="33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" s="37"/>
     </row>
@@ -1428,7 +1467,7 @@
     <row r="6" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="21"/>
       <c r="C6" s="28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
@@ -1447,15 +1486,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="21"/>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="84"/>
+      <c r="D8" s="88"/>
       <c r="E8" s="24"/>
-      <c r="F8" s="84" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="84"/>
+      <c r="F8" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="88"/>
       <c r="H8" s="20"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1507,7 +1546,7 @@
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="21"/>
       <c r="C13" s="22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="24"/>
@@ -1536,7 +1575,7 @@
     <row r="16" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="21"/>
       <c r="C16" s="28" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
@@ -1556,33 +1595,29 @@
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="21"/>
       <c r="C18" s="22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="5"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="20"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="21"/>
       <c r="C19" s="29" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="24"/>
-      <c r="F19" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="5"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
       <c r="H19" s="20"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="21"/>
       <c r="C20" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="24"/>
@@ -1611,7 +1646,7 @@
     <row r="23" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="21"/>
       <c r="C23" s="28" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D23" s="30"/>
       <c r="E23" s="24"/>
@@ -1631,7 +1666,7 @@
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
       <c r="C25" s="29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="24"/>
@@ -1660,7 +1695,7 @@
     <row r="28" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="21"/>
       <c r="C28" s="28" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="24"/>
@@ -1679,11 +1714,11 @@
     </row>
     <row r="30" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="21"/>
-      <c r="C30" s="81"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="82"/>
-      <c r="G30" s="83"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="86"/>
+      <c r="G30" s="87"/>
       <c r="H30" s="20"/>
     </row>
     <row r="31" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1700,7 +1735,7 @@
       <c r="D32" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="VoiU5WebjexVvjCjznz+vqdJJ0AoPPPHv+K9mx92vjqh7LcDvklWJmEtnoYaPhIp+7fnHWtBCBEPIx4GT1b48Q==" saltValue="1KfqEXaV6O7cJZ9lU1yD7g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="XWb1uwy1ExnRdFPkRj5azUK6n737P6b9od3enkYA6SHIwYpUh215KD916Pxa3f12lShq/c8+hWnKaW9OeMcOZg==" saltValue="lXh6uyEhLIklIU9ngl4aFg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="C30:G30"/>
     <mergeCell ref="C8:D8"/>
@@ -1708,7 +1743,7 @@
     <mergeCell ref="B2:H3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25 F19 C19:C20" xr:uid="{1EDF3C0A-2C62-4105-B534-7B9FBB507AE1}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25 C19:C20" xr:uid="{1EDF3C0A-2C62-4105-B534-7B9FBB507AE1}">
       <formula1>"&lt;0&gt;0"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1716,16 +1751,15 @@
     <hyperlink ref="C19" r:id="rId1" location="entities" xr:uid="{145A36E7-23E2-4F23-9423-3ABF5B1644A9}"/>
     <hyperlink ref="C20" r:id="rId2" location="countries" display="Flag country" xr:uid="{D830AF7F-6DD6-4CCC-B4E3-A0AB89AFD734}"/>
     <hyperlink ref="C25" r:id="rId3" location="types" xr:uid="{D5D73A23-873B-4484-A869-D712A7A31856}"/>
-    <hyperlink ref="F19" r:id="rId4" location="fisheries" xr:uid="{1FD9F71A-53CE-415C-90BB-4F39ADFA7B9E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C098252-FABC-4161-882E-794F98E79BC6}">
-  <dimension ref="B1:DD57"/>
+  <dimension ref="B1:DF57"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
@@ -1738,26 +1772,27 @@
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="48" customWidth="1"/>
-    <col min="6" max="6" width="10" style="50" customWidth="1"/>
-    <col min="7" max="7" width="10" style="51" customWidth="1"/>
-    <col min="8" max="8" width="12" style="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="72"/>
-    <col min="10" max="107" width="9.140625" style="73"/>
-    <col min="108" max="108" width="9.140625" style="74"/>
+    <col min="3" max="4" width="12.85546875" style="83" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="48" customWidth="1"/>
+    <col min="8" max="8" width="10" style="50" customWidth="1"/>
+    <col min="9" max="9" width="10" style="51" customWidth="1"/>
+    <col min="10" max="10" width="12" style="59" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="72"/>
+    <col min="12" max="109" width="9.140625" style="73"/>
+    <col min="110" max="110" width="9.140625" style="74"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:108" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:110" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="6"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
       <c r="G1" s="49"/>
-      <c r="H1"/>
-      <c r="I1"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
       <c r="J1"/>
       <c r="K1"/>
       <c r="L1"/>
@@ -1857,18 +1892,20 @@
       <c r="DB1"/>
       <c r="DC1"/>
       <c r="DD1"/>
-    </row>
-    <row r="2" spans="2:108" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="85" t="s">
+      <c r="DE1"/>
+      <c r="DF1"/>
+    </row>
+    <row r="2" spans="2:110" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
       <c r="J2" s="54"/>
       <c r="K2" s="54"/>
       <c r="L2" s="54"/>
@@ -1967,132 +2004,136 @@
       <c r="DA2" s="54"/>
       <c r="DB2" s="54"/>
       <c r="DC2" s="54"/>
-      <c r="DD2" s="55"/>
-    </row>
-    <row r="3" spans="2:108" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="94"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="91" t="s">
+      <c r="DD2" s="54"/>
+      <c r="DE2" s="54"/>
+      <c r="DF2" s="55"/>
+    </row>
+    <row r="3" spans="2:110" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
-      <c r="S3" s="92"/>
-      <c r="T3" s="92"/>
-      <c r="U3" s="92"/>
-      <c r="V3" s="92"/>
-      <c r="W3" s="92"/>
-      <c r="X3" s="92"/>
-      <c r="Y3" s="92"/>
-      <c r="Z3" s="92"/>
-      <c r="AA3" s="92"/>
-      <c r="AB3" s="92"/>
-      <c r="AC3" s="92"/>
-      <c r="AD3" s="92"/>
-      <c r="AE3" s="92"/>
-      <c r="AF3" s="92"/>
-      <c r="AG3" s="92"/>
-      <c r="AH3" s="92"/>
-      <c r="AI3" s="92"/>
-      <c r="AJ3" s="92"/>
-      <c r="AK3" s="92"/>
-      <c r="AL3" s="92"/>
-      <c r="AM3" s="92"/>
-      <c r="AN3" s="92"/>
-      <c r="AO3" s="92"/>
-      <c r="AP3" s="92"/>
-      <c r="AQ3" s="92"/>
-      <c r="AR3" s="92"/>
-      <c r="AS3" s="92"/>
-      <c r="AT3" s="92"/>
-      <c r="AU3" s="92"/>
-      <c r="AV3" s="92"/>
-      <c r="AW3" s="92"/>
-      <c r="AX3" s="92"/>
-      <c r="AY3" s="92"/>
-      <c r="AZ3" s="92"/>
-      <c r="BA3" s="92"/>
-      <c r="BB3" s="92"/>
-      <c r="BC3" s="92"/>
-      <c r="BD3" s="92"/>
-      <c r="BE3" s="92"/>
-      <c r="BF3" s="92"/>
-      <c r="BG3" s="92"/>
-      <c r="BH3" s="92"/>
-      <c r="BI3" s="92"/>
-      <c r="BJ3" s="92"/>
-      <c r="BK3" s="92"/>
-      <c r="BL3" s="92"/>
-      <c r="BM3" s="92"/>
-      <c r="BN3" s="92"/>
-      <c r="BO3" s="92"/>
-      <c r="BP3" s="92"/>
-      <c r="BQ3" s="92"/>
-      <c r="BR3" s="92"/>
-      <c r="BS3" s="92"/>
-      <c r="BT3" s="92"/>
-      <c r="BU3" s="92"/>
-      <c r="BV3" s="92"/>
-      <c r="BW3" s="92"/>
-      <c r="BX3" s="92"/>
-      <c r="BY3" s="92"/>
-      <c r="BZ3" s="92"/>
-      <c r="CA3" s="92"/>
-      <c r="CB3" s="92"/>
-      <c r="CC3" s="92"/>
-      <c r="CD3" s="92"/>
-      <c r="CE3" s="92"/>
-      <c r="CF3" s="92"/>
-      <c r="CG3" s="92"/>
-      <c r="CH3" s="92"/>
-      <c r="CI3" s="92"/>
-      <c r="CJ3" s="92"/>
-      <c r="CK3" s="92"/>
-      <c r="CL3" s="92"/>
-      <c r="CM3" s="92"/>
-      <c r="CN3" s="92"/>
-      <c r="CO3" s="92"/>
-      <c r="CP3" s="92"/>
-      <c r="CQ3" s="92"/>
-      <c r="CR3" s="92"/>
-      <c r="CS3" s="92"/>
-      <c r="CT3" s="92"/>
-      <c r="CU3" s="92"/>
-      <c r="CV3" s="92"/>
-      <c r="CW3" s="92"/>
-      <c r="CX3" s="92"/>
-      <c r="CY3" s="92"/>
-      <c r="CZ3" s="92"/>
-      <c r="DA3" s="92"/>
-      <c r="DB3" s="92"/>
-      <c r="DC3" s="92"/>
-      <c r="DD3" s="93"/>
-    </row>
-    <row r="4" spans="2:108" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
+      <c r="Q3" s="96"/>
+      <c r="R3" s="96"/>
+      <c r="S3" s="96"/>
+      <c r="T3" s="96"/>
+      <c r="U3" s="96"/>
+      <c r="V3" s="96"/>
+      <c r="W3" s="96"/>
+      <c r="X3" s="96"/>
+      <c r="Y3" s="96"/>
+      <c r="Z3" s="96"/>
+      <c r="AA3" s="96"/>
+      <c r="AB3" s="96"/>
+      <c r="AC3" s="96"/>
+      <c r="AD3" s="96"/>
+      <c r="AE3" s="96"/>
+      <c r="AF3" s="96"/>
+      <c r="AG3" s="96"/>
+      <c r="AH3" s="96"/>
+      <c r="AI3" s="96"/>
+      <c r="AJ3" s="96"/>
+      <c r="AK3" s="96"/>
+      <c r="AL3" s="96"/>
+      <c r="AM3" s="96"/>
+      <c r="AN3" s="96"/>
+      <c r="AO3" s="96"/>
+      <c r="AP3" s="96"/>
+      <c r="AQ3" s="96"/>
+      <c r="AR3" s="96"/>
+      <c r="AS3" s="96"/>
+      <c r="AT3" s="96"/>
+      <c r="AU3" s="96"/>
+      <c r="AV3" s="96"/>
+      <c r="AW3" s="96"/>
+      <c r="AX3" s="96"/>
+      <c r="AY3" s="96"/>
+      <c r="AZ3" s="96"/>
+      <c r="BA3" s="96"/>
+      <c r="BB3" s="96"/>
+      <c r="BC3" s="96"/>
+      <c r="BD3" s="96"/>
+      <c r="BE3" s="96"/>
+      <c r="BF3" s="96"/>
+      <c r="BG3" s="96"/>
+      <c r="BH3" s="96"/>
+      <c r="BI3" s="96"/>
+      <c r="BJ3" s="96"/>
+      <c r="BK3" s="96"/>
+      <c r="BL3" s="96"/>
+      <c r="BM3" s="96"/>
+      <c r="BN3" s="96"/>
+      <c r="BO3" s="96"/>
+      <c r="BP3" s="96"/>
+      <c r="BQ3" s="96"/>
+      <c r="BR3" s="96"/>
+      <c r="BS3" s="96"/>
+      <c r="BT3" s="96"/>
+      <c r="BU3" s="96"/>
+      <c r="BV3" s="96"/>
+      <c r="BW3" s="96"/>
+      <c r="BX3" s="96"/>
+      <c r="BY3" s="96"/>
+      <c r="BZ3" s="96"/>
+      <c r="CA3" s="96"/>
+      <c r="CB3" s="96"/>
+      <c r="CC3" s="96"/>
+      <c r="CD3" s="96"/>
+      <c r="CE3" s="96"/>
+      <c r="CF3" s="96"/>
+      <c r="CG3" s="96"/>
+      <c r="CH3" s="96"/>
+      <c r="CI3" s="96"/>
+      <c r="CJ3" s="96"/>
+      <c r="CK3" s="96"/>
+      <c r="CL3" s="96"/>
+      <c r="CM3" s="96"/>
+      <c r="CN3" s="96"/>
+      <c r="CO3" s="96"/>
+      <c r="CP3" s="96"/>
+      <c r="CQ3" s="96"/>
+      <c r="CR3" s="96"/>
+      <c r="CS3" s="96"/>
+      <c r="CT3" s="96"/>
+      <c r="CU3" s="96"/>
+      <c r="CV3" s="96"/>
+      <c r="CW3" s="96"/>
+      <c r="CX3" s="96"/>
+      <c r="CY3" s="96"/>
+      <c r="CZ3" s="96"/>
+      <c r="DA3" s="96"/>
+      <c r="DB3" s="96"/>
+      <c r="DC3" s="96"/>
+      <c r="DD3" s="96"/>
+      <c r="DE3" s="96"/>
+      <c r="DF3" s="97"/>
+    </row>
+    <row r="4" spans="2:110" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="53"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
       <c r="E4" s="56"/>
       <c r="F4" s="56"/>
       <c r="G4" s="56"/>
-      <c r="H4" s="77" t="s">
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
+      <c r="K4" s="60"/>
       <c r="L4" s="61"/>
       <c r="M4" s="61"/>
       <c r="N4" s="61"/>
@@ -2189,21 +2230,23 @@
       <c r="DA4" s="61"/>
       <c r="DB4" s="61"/>
       <c r="DC4" s="61"/>
-      <c r="DD4" s="62"/>
-    </row>
-    <row r="5" spans="2:108" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="DD4" s="61"/>
+      <c r="DE4" s="61"/>
+      <c r="DF4" s="62"/>
+    </row>
+    <row r="5" spans="2:110" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="53"/>
       <c r="C5" s="56"/>
       <c r="D5" s="56"/>
       <c r="E5" s="56"/>
       <c r="F5" s="56"/>
       <c r="G5" s="56"/>
-      <c r="H5" s="78" t="s">
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="63"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
+      <c r="K5" s="63"/>
       <c r="L5" s="64"/>
       <c r="M5" s="64"/>
       <c r="N5" s="64"/>
@@ -2300,25 +2343,27 @@
       <c r="DA5" s="64"/>
       <c r="DB5" s="64"/>
       <c r="DC5" s="64"/>
-      <c r="DD5" s="65"/>
-    </row>
-    <row r="6" spans="2:108" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="96" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="96" t="s">
+      <c r="DD5" s="64"/>
+      <c r="DE5" s="64"/>
+      <c r="DF5" s="65"/>
+    </row>
+    <row r="6" spans="2:110" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="97"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="76" t="s">
+      <c r="H6" s="101"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="63"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
+      <c r="K6" s="63"/>
       <c r="L6" s="64"/>
       <c r="M6" s="64"/>
       <c r="N6" s="64"/>
@@ -2415,33 +2460,39 @@
       <c r="DA6" s="64"/>
       <c r="DB6" s="64"/>
       <c r="DC6" s="64"/>
-      <c r="DD6" s="65"/>
-    </row>
-    <row r="7" spans="2:108" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="DD6" s="64"/>
+      <c r="DE6" s="64"/>
+      <c r="DF6" s="65"/>
+    </row>
+    <row r="7" spans="2:110" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="D7" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="F7" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="G7" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="80" t="s">
+      <c r="H7" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="52" t="s">
+      <c r="I7" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="79" t="s">
+      <c r="J7" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="66"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
+      <c r="K7" s="66"/>
       <c r="L7" s="67"/>
       <c r="M7" s="67"/>
       <c r="N7" s="67"/>
@@ -2538,19 +2589,21 @@
       <c r="DA7" s="67"/>
       <c r="DB7" s="67"/>
       <c r="DC7" s="67"/>
-      <c r="DD7" s="68"/>
-    </row>
-    <row r="8" spans="2:108" x14ac:dyDescent="0.25">
+      <c r="DD7" s="67"/>
+      <c r="DE7" s="67"/>
+      <c r="DF7" s="68"/>
+    </row>
+    <row r="8" spans="2:110" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="69"/>
       <c r="L8" s="70"/>
       <c r="M8" s="70"/>
       <c r="N8" s="70"/>
@@ -2647,432 +2700,533 @@
       <c r="DA8" s="70"/>
       <c r="DB8" s="70"/>
       <c r="DC8" s="70"/>
-      <c r="DD8" s="71"/>
-    </row>
-    <row r="9" spans="2:108" x14ac:dyDescent="0.25">
+      <c r="DD8" s="70"/>
+      <c r="DE8" s="70"/>
+      <c r="DF8" s="71"/>
+    </row>
+    <row r="9" spans="2:110" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="43"/>
-    </row>
-    <row r="10" spans="2:108" x14ac:dyDescent="0.25">
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="43"/>
+    </row>
+    <row r="10" spans="2:110" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="43"/>
-    </row>
-    <row r="11" spans="2:108" x14ac:dyDescent="0.25">
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="43"/>
+    </row>
+    <row r="11" spans="2:110" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="43"/>
-    </row>
-    <row r="12" spans="2:108" x14ac:dyDescent="0.25">
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="43"/>
+    </row>
+    <row r="12" spans="2:110" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="43"/>
-    </row>
-    <row r="13" spans="2:108" x14ac:dyDescent="0.25">
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="43"/>
+    </row>
+    <row r="13" spans="2:110" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="43"/>
-    </row>
-    <row r="14" spans="2:108" x14ac:dyDescent="0.25">
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="43"/>
+    </row>
+    <row r="14" spans="2:110" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="43"/>
-    </row>
-    <row r="15" spans="2:108" x14ac:dyDescent="0.25">
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="43"/>
+    </row>
+    <row r="15" spans="2:110" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="43"/>
-    </row>
-    <row r="16" spans="2:108" x14ac:dyDescent="0.25">
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="43"/>
+    </row>
+    <row r="16" spans="2:110" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="43"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="82"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="43"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="43"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="82"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="43"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="43"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="82"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="43"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="43"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="43"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="43"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="82"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="43"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="43"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="43"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="43"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="43"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="43"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="82"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="43"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="43"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="43"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="43"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="82"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="43"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="43"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="43"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="43"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="43"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="43"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="43"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="43"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="82"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="43"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="43"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="43"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="43"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="43"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="43"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="82"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="43"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="43"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="82"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="43"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="43"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="82"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="43"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="43"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="82"/>
+      <c r="D35" s="82"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="43"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="43"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="43"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="43"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="43"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="43"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="43"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="43"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="43"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="43"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="82"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="43"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="43"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="82"/>
+      <c r="D41" s="82"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="41"/>
+      <c r="I41" s="43"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="43"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="82"/>
+      <c r="D42" s="82"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="43"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="43"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="82"/>
+      <c r="D43" s="82"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="43"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="43"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="82"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="43"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="43"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="82"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="43"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="7"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="43"/>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="82"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="43"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="7"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="43"/>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="82"/>
+      <c r="D47" s="82"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="43"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="43"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C48" s="82"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="41"/>
+      <c r="I48" s="43"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="43"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="82"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="43"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="43"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C50" s="82"/>
+      <c r="D50" s="82"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="43"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="7"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="39"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="43"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C51" s="82"/>
+      <c r="D51" s="82"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="43"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="41"/>
-      <c r="G52" s="43"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C52" s="82"/>
+      <c r="D52" s="82"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="43"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="7"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="43"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C53" s="82"/>
+      <c r="D53" s="82"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="43"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="39"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="43"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C54" s="82"/>
+      <c r="D54" s="82"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="41"/>
+      <c r="I54" s="43"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="7"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="41"/>
-      <c r="G55" s="43"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C55" s="82"/>
+      <c r="D55" s="82"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="41"/>
+      <c r="I55" s="43"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="43"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C56" s="82"/>
+      <c r="D56" s="82"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="41"/>
+      <c r="I56" s="43"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="7"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="39"/>
-      <c r="F57" s="41"/>
-      <c r="G57" s="43"/>
+      <c r="C57" s="82"/>
+      <c r="D57" s="82"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="41"/>
+      <c r="I57" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="uPodclcUZ3mTHXNJFrNv5UeCyq1mkIOiJg9kBXWyFkUE9vAY+liw52pu9BayEjaAvodeM3mNHE7jlUnodPIKcg==" saltValue="OJ4eVIGD+ICJgTlZ7js1ag==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="IhkS4ZZGrC0apCJlXugchWySxz5yhMBN2Co7XzWa9fui5GUbL0KJ3JyWZ/kH/6y3Zd2Pz/UGEC76hXyqb69vrA==" saltValue="2IsUyBOe93s6rv3V5cnssw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="4">
-    <mergeCell ref="I3:DD3"/>
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="K3:DF3"/>
+    <mergeCell ref="B2:I3"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="G6:I6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B8:G1048576">
+  <conditionalFormatting sqref="B8:I1048576">
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>B8=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:DD1048576">
+  <conditionalFormatting sqref="K8:DF1048576">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>I8=""</formula>
+      <formula>K8=""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7 G7 H4:H7" xr:uid="{86B40B65-30E0-465F-9E4E-BDD2D0A3ECB3}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7 I7 J4:J7 D7" xr:uid="{86B40B65-30E0-465F-9E4E-BDD2D0A3ECB3}">
       <formula1>"&lt;0&gt;0"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1" location="FOBactivityTypes" xr:uid="{3C4B7339-15DC-4AE3-BA6F-6F6FE197BAF1}"/>
-    <hyperlink ref="F7" r:id="rId2" location="FOBtypes" xr:uid="{0D9BDFCB-0E93-45FA-A9F8-2F2F4961FF03}"/>
-    <hyperlink ref="H4" r:id="rId3" location="allSpecies" xr:uid="{C9772F96-5988-4592-A714-5A7067090A05}"/>
-    <hyperlink ref="H5" r:id="rId4" location="typesOfFate" xr:uid="{8E08F5E0-486B-464D-9A3A-733FD4CA38A4}"/>
-    <hyperlink ref="H7" r:id="rId5" location="catchUnits" xr:uid="{9192771E-64B4-4C0E-959B-793135738F4C}"/>
-    <hyperlink ref="H6" r:id="rId6" location="raisings" xr:uid="{C0444C52-8B48-4E54-9861-D973CED3CDC3}"/>
+    <hyperlink ref="I7" r:id="rId1" location="FOBactivityTypes" xr:uid="{3C4B7339-15DC-4AE3-BA6F-6F6FE197BAF1}"/>
+    <hyperlink ref="H7" r:id="rId2" location="FOBtypes" xr:uid="{0D9BDFCB-0E93-45FA-A9F8-2F2F4961FF03}"/>
+    <hyperlink ref="J4" r:id="rId3" location="allSpecies" xr:uid="{C9772F96-5988-4592-A714-5A7067090A05}"/>
+    <hyperlink ref="J5" r:id="rId4" location="typesOfFate" xr:uid="{8E08F5E0-486B-464D-9A3A-733FD4CA38A4}"/>
+    <hyperlink ref="J7" r:id="rId5" location="catchUnits" xr:uid="{9192771E-64B4-4C0E-959B-793135738F4C}"/>
+    <hyperlink ref="J6" r:id="rId6" location="raisings" xr:uid="{C0444C52-8B48-4E54-9861-D973CED3CDC3}"/>
+    <hyperlink ref="D7" r:id="rId7" location="fisheries" xr:uid="{9B90DF27-D07F-4162-B42D-F8BE1A2C0F3E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>